<commit_message>
Updated ppt, mpp, and xls
</commit_message>
<xml_diff>
--- a/Team Deliverable 1/Gantt chart for pres.xlsx
+++ b/Team Deliverable 1/Gantt chart for pres.xlsx
@@ -347,8 +347,8 @@
               <c:idx val="0"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-4.5289112320021634E-2"/>
-                  <c:y val="-5.2601919008275183E-2"/>
+                  <c:x val="0.17090224002588453"/>
+                  <c:y val="-5.5340894631392114E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:dLblPos val="r"/>
@@ -382,7 +382,7 @@
                   <c:v>42418</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42424</c:v>
+                  <c:v>42462</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -522,7 +522,7 @@
               <c:idx val="1"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.2876840831878536"/>
+                  <c:x val="-0.39961293936693981"/>
                   <c:y val="-5.2602134675647054E-2"/>
                 </c:manualLayout>
               </c:layout>
@@ -1086,11 +1086,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="156756224"/>
-        <c:axId val="156755648"/>
+        <c:axId val="791939328"/>
+        <c:axId val="791939904"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="156756224"/>
+        <c:axId val="791939328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1110,12 +1110,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="156755648"/>
+        <c:crossAx val="791939904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="156755648"/>
+        <c:axId val="791939904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1132,7 +1132,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="156756224"/>
+        <c:crossAx val="791939328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1480,7 +1480,7 @@
   <dimension ref="A3:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1546,7 +1546,7 @@
         <v>5</v>
       </c>
       <c r="E5" s="5">
-        <v>42424</v>
+        <v>42462</v>
       </c>
       <c r="F5" s="10">
         <v>5</v>

</xml_diff>